<commit_message>
update correction and processed data from update_data
</commit_message>
<xml_diff>
--- a/data/2020-07-08/tn.xlsx
+++ b/data/2020-07-08/tn.xlsx
@@ -10,7 +10,7 @@
     <sheet sheetId="1" r:id="rId1" name="ALL_AGE_FINAL"/>
   </sheets>
   <definedNames>
-    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$1109</definedName>
+    <definedName name="ALL_AGE_FINAL">'ALL_AGE_FINAL'!$A$1:$H$1099</definedName>
   </definedNames>
   <calcPr calcId="125725" fullCalcOnLoad="true"/>
 </workbook>
@@ -347,7 +347,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H1109"/>
+  <dimension ref="A1:H1099"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
       <selection activeCell="C5" sqref="C5"/>
@@ -29863,286 +29863,6 @@
         <v>0</v>
       </c>
     </row>
-    <row outlineLevel="0" r="1100">
-      <c r="A1100" s="1">
-        <v>44020</v>
-      </c>
-      <c r="B1100" s="0" t="inlineStr">
-        <is>
-          <t>0-10 years</t>
-        </is>
-      </c>
-      <c r="C1100" s="0">
-        <v>2558</v>
-      </c>
-      <c r="D1100" s="0">
-        <v>4.56899939270532E-02</v>
-      </c>
-      <c r="E1100" s="0">
-        <v>114</v>
-      </c>
-      <c r="F1100" s="0">
-        <v>4.61165048543689E-02</v>
-      </c>
-      <c r="G1100" s="0">
-        <v>3</v>
-      </c>
-      <c r="H1100" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="1101">
-      <c r="A1101" s="1">
-        <v>44020</v>
-      </c>
-      <c r="B1101" s="0" t="inlineStr">
-        <is>
-          <t>11-20 years</t>
-        </is>
-      </c>
-      <c r="C1101" s="0">
-        <v>5611</v>
-      </c>
-      <c r="D1101" s="0">
-        <v>0.100221483942414</v>
-      </c>
-      <c r="E1101" s="0">
-        <v>292</v>
-      </c>
-      <c r="F1101" s="0">
-        <v>0.118122977346278</v>
-      </c>
-      <c r="G1101" s="0">
-        <v>0</v>
-      </c>
-      <c r="H1101" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="1102">
-      <c r="A1102" s="1">
-        <v>44020</v>
-      </c>
-      <c r="B1102" s="0" t="inlineStr">
-        <is>
-          <t>21-30 years</t>
-        </is>
-      </c>
-      <c r="C1102" s="0">
-        <v>13150</v>
-      </c>
-      <c r="D1102" s="0">
-        <v>0.234880148608581</v>
-      </c>
-      <c r="E1102" s="0">
-        <v>687</v>
-      </c>
-      <c r="F1102" s="0">
-        <v>0.277912621359223</v>
-      </c>
-      <c r="G1102" s="0">
-        <v>9</v>
-      </c>
-      <c r="H1102" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="1103">
-      <c r="A1103" s="1">
-        <v>44020</v>
-      </c>
-      <c r="B1103" s="0" t="inlineStr">
-        <is>
-          <t>31-40 years</t>
-        </is>
-      </c>
-      <c r="C1103" s="0">
-        <v>11084</v>
-      </c>
-      <c r="D1103" s="0">
-        <v>0.197978065945058</v>
-      </c>
-      <c r="E1103" s="0">
-        <v>445</v>
-      </c>
-      <c r="F1103" s="0">
-        <v>0.180016181229773</v>
-      </c>
-      <c r="G1103" s="0">
-        <v>12</v>
-      </c>
-      <c r="H1103" s="0">
-        <v>-1</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="1104">
-      <c r="A1104" s="1">
-        <v>44020</v>
-      </c>
-      <c r="B1104" s="0" t="inlineStr">
-        <is>
-          <t>41-50 years</t>
-        </is>
-      </c>
-      <c r="C1104" s="0">
-        <v>9069</v>
-      </c>
-      <c r="D1104" s="0">
-        <v>0.161986925302754</v>
-      </c>
-      <c r="E1104" s="0">
-        <v>367</v>
-      </c>
-      <c r="F1104" s="0">
-        <v>0.148462783171521</v>
-      </c>
-      <c r="G1104" s="0">
-        <v>32</v>
-      </c>
-      <c r="H1104" s="0">
-        <v>0</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="1105">
-      <c r="A1105" s="1">
-        <v>44020</v>
-      </c>
-      <c r="B1105" s="0" t="inlineStr">
-        <is>
-          <t>51-60 years</t>
-        </is>
-      </c>
-      <c r="C1105" s="0">
-        <v>7008</v>
-      </c>
-      <c r="D1105" s="0">
-        <v>0.125174150680527</v>
-      </c>
-      <c r="E1105" s="0">
-        <v>266</v>
-      </c>
-      <c r="F1105" s="0">
-        <v>0.107605177993528</v>
-      </c>
-      <c r="G1105" s="0">
-        <v>66</v>
-      </c>
-      <c r="H1105" s="0">
-        <v>1</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="1106">
-      <c r="A1106" s="1">
-        <v>44020</v>
-      </c>
-      <c r="B1106" s="0" t="inlineStr">
-        <is>
-          <t>61-70 years</t>
-        </is>
-      </c>
-      <c r="C1106" s="0">
-        <v>4015</v>
-      </c>
-      <c r="D1106" s="0">
-        <v>7.17143571607188E-02</v>
-      </c>
-      <c r="E1106" s="0">
-        <v>160</v>
-      </c>
-      <c r="F1106" s="0">
-        <v>6.47249190938511E-02</v>
-      </c>
-      <c r="G1106" s="0">
-        <v>128</v>
-      </c>
-      <c r="H1106" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="1107">
-      <c r="A1107" s="1">
-        <v>44020</v>
-      </c>
-      <c r="B1107" s="0" t="inlineStr">
-        <is>
-          <t>71-80 years</t>
-        </is>
-      </c>
-      <c r="C1107" s="0">
-        <v>2060</v>
-      </c>
-      <c r="D1107" s="0">
-        <v>3.67949130139678E-02</v>
-      </c>
-      <c r="E1107" s="0">
-        <v>73</v>
-      </c>
-      <c r="F1107" s="0">
-        <v>2.95307443365696E-02</v>
-      </c>
-      <c r="G1107" s="0">
-        <v>208</v>
-      </c>
-      <c r="H1107" s="0">
-        <v>8</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="1108">
-      <c r="A1108" s="1">
-        <v>44020</v>
-      </c>
-      <c r="B1108" s="0" t="inlineStr">
-        <is>
-          <t>81+ years</t>
-        </is>
-      </c>
-      <c r="C1108" s="0">
-        <v>1183</v>
-      </c>
-      <c r="D1108" s="0">
-        <v>2.11302825706427E-02</v>
-      </c>
-      <c r="E1108" s="0">
-        <v>39</v>
-      </c>
-      <c r="F1108" s="0">
-        <v>1.57766990291262E-02</v>
-      </c>
-      <c r="G1108" s="0">
-        <v>227</v>
-      </c>
-      <c r="H1108" s="0">
-        <v>7</v>
-      </c>
-    </row>
-    <row outlineLevel="0" r="1109">
-      <c r="A1109" s="1">
-        <v>44020</v>
-      </c>
-      <c r="B1109" s="0" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="C1109" s="0">
-        <v>248</v>
-      </c>
-      <c r="D1109" s="0">
-        <v>4.4296788482835E-03</v>
-      </c>
-      <c r="E1109" s="0">
-        <v>29</v>
-      </c>
-      <c r="F1109" s="0">
-        <v>1.17313915857605E-02</v>
-      </c>
-      <c r="G1109" s="0">
-        <v>0</v>
-      </c>
-      <c r="H1109" s="0">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>